<commit_message>
vault backup: 2024-01-19 13:52:16
Affected files:
.obsidian/graph.json
.obsidian/workspace.json
Notatki/Semestr 3/Architektura komputerów 1/Ćwiczenia/Kolokwium/Drawing 2024-01-18 09.17.08.excalidraw.md
Notatki/Semestr 3/Architektura komputerów 1/Ćwiczenia/Kolokwium/Drawing 2024-01-18 09.17.08.excalidraw.svg
Notatki/Semestr 3/Inżynierskie zastosowania statystyki/Ćwiczenia/Kolokwium 2/IZS kolos.xlsx
Notatki/Semestr 3/Logika układów cyfrowych/Wykłady/Wykłady.md
</commit_message>
<xml_diff>
--- a/Notatki/Semestr 3/Inżynierskie zastosowania statystyki/Ćwiczenia/Kolokwium 2/IZS kolos.xlsx
+++ b/Notatki/Semestr 3/Inżynierskie zastosowania statystyki/Ćwiczenia/Kolokwium 2/IZS kolos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xeder\Documents\notes\Studia\Notatki\Semestr 3\Inżynierskie zastosowania statystyki\Ćwiczenia\Kolokwium 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE29DF6-8C6D-439D-A05B-1930438C80E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C463E7B-DBD0-4108-945F-AA94855CE5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="9" xr2:uid="{EEEA31D6-0E80-4109-8014-5AC21CA1198A}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>średnia</t>
   </si>
@@ -262,6 +262,21 @@
   </si>
   <si>
     <t>rozkłądy</t>
+  </si>
+  <si>
+    <t>nieobciążone</t>
+  </si>
+  <si>
+    <t>zakładamy ze rowne</t>
+  </si>
+  <si>
+    <t>zakładamy ze równe</t>
+  </si>
+  <si>
+    <t>zakładamy ze niezależne</t>
+  </si>
+  <si>
+    <t>do inf obszar krytyczny</t>
   </si>
 </sst>
 </file>
@@ -355,6 +370,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>368796</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>101788</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obraz 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC6E42C-1EE7-7005-BD38-76028A784BD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3117850" y="311150"/>
+          <a:ext cx="9652496" cy="3657788"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -706,7 +770,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -749,6 +813,17 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3.7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" cm="1">
+        <f t="array" ref="G3">SUMSQ(A2:A6-F2)/(COUNTA(A2:A6)-1)</f>
+        <v>0.628</v>
+      </c>
+      <c r="H3">
+        <f>SQRT(G3)</f>
+        <v>0.792464510246358</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -779,7 +854,7 @@
   <dimension ref="A1:P100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -898,23 +973,23 @@
         <v>30</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C10" si="0">A7-$A$2</f>
+        <f>A7-$A$2</f>
         <v>-1</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D10" si="1">B7-$B$2</f>
+        <f t="shared" ref="D7:D10" si="0">B7-$B$2</f>
         <v>-10</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E70" si="2">C7*D7</f>
+        <f t="shared" ref="E7:E70" si="1">C7*D7</f>
         <v>10</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F70" si="3">C7^2</f>
+        <f t="shared" ref="F7:F70" si="2">C7^2</f>
         <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G70" si="4">D7^2</f>
+        <f t="shared" ref="G7:G70" si="3">D7^2</f>
         <v>100</v>
       </c>
       <c r="J7" t="s">
@@ -936,23 +1011,23 @@
         <v>40</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C7:C10" si="4">A8-$A$2</f>
         <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L8" s="2"/>
@@ -965,23 +1040,23 @@
         <v>50</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="J9" t="s">
@@ -996,23 +1071,23 @@
         <v>50</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="J10" t="s">
@@ -1025,15 +1100,15 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J11" t="s">
@@ -1046,169 +1121,169 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L23">
@@ -1222,15 +1297,15 @@
     </row>
     <row r="24" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L24">
@@ -1240,71 +1315,71 @@
     </row>
     <row r="25" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M29" t="s">
@@ -1323,15 +1398,15 @@
     </row>
     <row r="30" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N30">
@@ -1343,15 +1418,15 @@
     </row>
     <row r="31" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M31" t="s">
@@ -1366,15 +1441,15 @@
     </row>
     <row r="32" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N32">
@@ -1389,15 +1464,15 @@
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N33">
@@ -1412,519 +1487,519 @@
     </row>
     <row r="34" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F62">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2360,10 +2435,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2376,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1300</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2384,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>500</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2392,7 +2467,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2400,7 +2475,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1200</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2409,7 +2484,12 @@
       </c>
       <c r="B6">
         <f>(B1-B4)*SQRT(B3)/B2</f>
-        <v>2</v>
+        <v>0.84852813742385691</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2422,10 +2502,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2485,8 +2565,14 @@
         <v>2.1438645980253872</v>
       </c>
     </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2495,10 +2581,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="E12:H18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2512,13 +2598,13 @@
         <v>12</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>6.65</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
       </c>
       <c r="E1">
-        <v>2.5</v>
+        <v>6.36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -2526,15 +2612,13 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <f>0.9^2</f>
-        <v>0.81</v>
+        <v>0.05</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2">
-        <f>0.5^2</f>
-        <v>0.25</v>
+        <v>0.06</v>
       </c>
       <c r="I2" t="s">
         <v>15</v>
@@ -2545,13 +2629,13 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
@@ -2570,7 +2654,12 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C7">
         <f>(B1-E1)/(SQRT((B2/B3)+(E2/E3)))</f>
-        <v>3.9528470752104745</v>
+        <v>2.7650415088122178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2583,10 +2672,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2613,7 +2702,6 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <f>10^2</f>
         <v>100</v>
       </c>
       <c r="D2" t="s">
@@ -2656,8 +2744,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C7">
-        <f>(B1-E1)/(SQRT((B3*B2+E3*E2/(B3+E3-2))*((1/B3)+(1/E3))))</f>
-        <v>-1.4635001432602284</v>
+        <f>(B1-E1)/(SQRT(((B3*B2+E3*E2)/(B3+E3-2))*((1/B3)+(1/E3))))</f>
+        <v>-3.9191835884530843</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2673,7 +2766,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2732,8 +2825,8 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C7">
-        <f>(B1-E1)/(SQRT((B3*B2+E3*E2/(B3+E3-2))*((1/B3)+(1/E3))))</f>
-        <v>-1.4635001432602284</v>
+        <f>(B1-E1)/(SQRT(((B3*B2+E3*E2)/(B3+E3-2))*((1/B3)+(1/E3))))</f>
+        <v>-3.9191835884530843</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2754,7 +2847,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2808,32 +2901,32 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2">
         <f>$I2*B$9/$I$9</f>
-        <v>3.9666666666666668</v>
+        <v>22.065217391304348</v>
       </c>
       <c r="O2">
         <f t="shared" ref="O2:T2" si="0">$I2*C$9/$I$9</f>
-        <v>6.5166666666666666</v>
+        <v>5.0434782608695654</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>6.5166666666666666</v>
+        <v>1.8913043478260869</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
@@ -2857,32 +2950,32 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I7" si="1">SUM(B3:H3)</f>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N8" si="2">$I3*B$9/$I$9</f>
-        <v>5.1333333333333337</v>
+        <v>9.1304347826086953</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O8" si="3">$I3*C$9/$I$9</f>
-        <v>8.4333333333333336</v>
+        <v>2.0869565217391304</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P8" si="4">$I3*D$9/$I$9</f>
-        <v>8.4333333333333336</v>
+        <v>0.78260869565217395</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q8" si="5">$I3*E$9/$I$9</f>
@@ -2906,32 +2999,32 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="M4">
         <v>3</v>
       </c>
       <c r="N4">
         <f t="shared" si="2"/>
-        <v>4.9000000000000004</v>
+        <v>3.8043478260869565</v>
       </c>
       <c r="O4">
         <f t="shared" si="3"/>
-        <v>8.0500000000000007</v>
+        <v>0.86956521739130432</v>
       </c>
       <c r="P4">
         <f t="shared" si="4"/>
-        <v>8.0500000000000007</v>
+        <v>0.32608695652173914</v>
       </c>
       <c r="Q4">
         <f t="shared" si="5"/>
@@ -3113,15 +3206,15 @@
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B9">
         <f>SUM(B2:B8)</f>
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:H9" si="9">SUM(C2:C8)</f>
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <f t="shared" si="9"/>
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <f t="shared" si="9"/>
@@ -3141,21 +3234,21 @@
       </c>
       <c r="I9">
         <f>SUM(B2:H8)</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.35">
       <c r="J18">
         <f>IF(N2&lt;&gt;0,((B2-N2)^2/N2),0)</f>
-        <v>6.3868347338935569</v>
+        <v>0.19329620903833794</v>
       </c>
       <c r="K18">
         <f t="shared" ref="K18:P18" si="10">IF(O2&lt;&gt;0,((C2-O2)^2/O2),0)</f>
-        <v>0.35298380221653874</v>
+        <v>0.18140929535232375</v>
       </c>
       <c r="L18">
         <f t="shared" si="10"/>
-        <v>1.8977408354646206</v>
+        <v>0.6499250374812594</v>
       </c>
       <c r="M18">
         <f t="shared" si="10"/>
@@ -3174,18 +3267,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.35">
       <c r="J19">
         <f t="shared" ref="J19:J24" si="11">IF(N3&lt;&gt;0,((B3-N3)^2/N3),0)</f>
-        <v>0.25021645021645039</v>
+        <v>8.2815734989648102E-2</v>
       </c>
       <c r="K19">
         <f t="shared" ref="K19:K24" si="12">IF(O3&lt;&gt;0,((C3-O3)^2/O3),0)</f>
-        <v>1.5084321475625821</v>
+        <v>3.6231884057970967E-3</v>
       </c>
       <c r="L19">
         <f t="shared" ref="L19:L24" si="13">IF(P3&lt;&gt;0,((D3-P3)^2/P3),0)</f>
-        <v>0.70210803689064571</v>
+        <v>0.78260869565217395</v>
       </c>
       <c r="M19">
         <f t="shared" ref="M19:M24" si="14">IF(Q3&lt;&gt;0,((E3-Q3)^2/Q3),0)</f>
@@ -3204,18 +3297,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.35">
       <c r="J20">
         <f t="shared" si="11"/>
-        <v>3.1040816326530614</v>
+        <v>0.37577639751552794</v>
       </c>
       <c r="K20">
         <f t="shared" si="12"/>
-        <v>0.52204968944099417</v>
+        <v>0.86956521739130432</v>
       </c>
       <c r="L20">
         <f t="shared" si="13"/>
-        <v>4.3978260869565204</v>
+        <v>0.32608695652173914</v>
       </c>
       <c r="M20">
         <f t="shared" si="14"/>
@@ -3234,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:18" x14ac:dyDescent="0.35">
       <c r="J21">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3264,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>63</v>
       </c>
@@ -3297,7 +3390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>61</v>
       </c>
@@ -3330,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:18" x14ac:dyDescent="0.35">
       <c r="J24">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3360,16 +3453,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.35">
       <c r="P25" t="s">
         <v>28</v>
       </c>
       <c r="Q25">
         <f>SUM(J18:P24)</f>
-        <v>19.12227341529497</v>
-      </c>
-    </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.35">
+        <v>3.465106732348112</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.35">
       <c r="P26" t="s">
         <v>27</v>
       </c>
@@ -3377,8 +3470,11 @@
         <f>(COUNTA(B2:H2)-1)*(COUNTA(B2:B8)-1)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="R26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.35">
       <c r="P27" t="s">
         <v>29</v>
       </c>
@@ -3393,7 +3489,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -3465,6 +3561,11 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I23" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3480,12 +3581,13 @@
   <dimension ref="A3:F100"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -3501,7 +3603,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6">
         <f xml:space="preserve"> SUM(B8:B100)</f>
-        <v>740</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -3530,7 +3632,7 @@
         <v>39</v>
       </c>
       <c r="B8">
-        <v>200</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <f>1/5</f>
@@ -3538,15 +3640,15 @@
       </c>
       <c r="D8">
         <f>C8*$B$6</f>
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="E8">
         <f>IF(D8&lt;&gt;0,(B8-D8)^2/D8,0)</f>
-        <v>18.27027027027027</v>
+        <v>2.5714285714285716</v>
       </c>
       <c r="F8">
         <f>SUM(E8:E13)</f>
-        <v>35.675675675675677</v>
+        <v>18.285714285714285</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -3554,7 +3656,7 @@
         <v>40</v>
       </c>
       <c r="B9">
-        <v>160</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <f>1/5</f>
@@ -3562,11 +3664,11 @@
       </c>
       <c r="D9">
         <f t="shared" ref="D9:D72" si="0">C9*$B$6</f>
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="E9">
         <f t="shared" ref="E9:E72" si="1">IF(D9&lt;&gt;0,(B9-D9)^2/D9,0)</f>
-        <v>0.97297297297297303</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -3574,7 +3676,7 @@
         <v>41</v>
       </c>
       <c r="B10">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <f>1/5</f>
@@ -3582,11 +3684,11 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>0.43243243243243246</v>
+        <v>1.1428571428571428</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -3594,7 +3696,7 @@
         <v>42</v>
       </c>
       <c r="B11">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <f t="shared" ref="C11:C12" si="2">1/5</f>
@@ -3602,11 +3704,11 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>0.43243243243243246</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3614,7 +3716,7 @@
         <v>43</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <f t="shared" si="2"/>
@@ -3622,11 +3724,11 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>15.567567567567568</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>